<commit_message>
psp update, sad upload
</commit_message>
<xml_diff>
--- a/5조_PSP.xlsx
+++ b/5조_PSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hye Min\Documents\GitHub\pumasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF68A43-5C6A-4440-999A-57BE0A01B9DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC6A097-4FAE-4E56-B040-FB7C8D6652FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="107">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -3561,7 +3561,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4144,12 +4144,24 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="4"/>
+      <c r="A32" s="13">
+        <v>43781</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>60</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
@@ -7007,11 +7019,11 @@
       </c>
       <c r="C15" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A15,김혜민!E:E)+SUMIF('김백준(휴학)'!F:F,TOTAL!A15,'김백준(휴학)'!E:E)+SUMIF(박진근!F:F,TOTAL!A15,박진근!E:E)+SUMIF(이미정!F:F,TOTAL!A15,이미정!E:E)+SUMIF(정동연!F:F,TOTAL!A15,정동연!E:E)+SUMIF(탁재인!F:F,TOTAL!A15,탁재인!E:E)</f>
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="D15" s="37">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="E15" s="42" t="s">
         <v>97</v>

</xml_diff>

<commit_message>
Mijeong PSP update _ 11/23
</commit_message>
<xml_diff>
--- a/5조_PSP.xlsx
+++ b/5조_PSP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hye Min\pumasi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이미정\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD13007-9703-40DC-8AC6-E94FD76C6C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78427F24-6E1D-4573-AC80-266A28010AA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="975" windowWidth="15660" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1512" yWindow="768" windowWidth="10824" windowHeight="10932" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="김혜민" sheetId="1" r:id="rId1"/>
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="114">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2976,6 +2976,10 @@
       </rPr>
       <t>로직짜기</t>
     </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -3643,20 +3647,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3668,10 +3672,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -3683,8 +3687,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -3725,7 +3729,7 @@
       </c>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43713</v>
       </c>
@@ -3746,7 +3750,7 @@
       </c>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43714</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>43715</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>43717</v>
       </c>
@@ -3806,7 +3810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>43725</v>
       </c>
@@ -3826,7 +3830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>43726</v>
       </c>
@@ -3846,7 +3850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>43727</v>
       </c>
@@ -3866,7 +3870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>43728</v>
       </c>
@@ -3886,7 +3890,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>43728</v>
       </c>
@@ -3906,7 +3910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>43728</v>
       </c>
@@ -3926,7 +3930,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>43730</v>
       </c>
@@ -3946,7 +3950,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>43735</v>
       </c>
@@ -3966,7 +3970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>43736</v>
       </c>
@@ -3986,7 +3990,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>43736</v>
       </c>
@@ -4006,7 +4010,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>43742</v>
       </c>
@@ -4026,7 +4030,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>43745</v>
       </c>
@@ -4046,7 +4050,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>43745</v>
       </c>
@@ -4066,7 +4070,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>43747</v>
       </c>
@@ -4086,7 +4090,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>43748</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43749</v>
       </c>
@@ -4126,7 +4130,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>43764</v>
       </c>
@@ -4146,7 +4150,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>43764</v>
       </c>
@@ -4166,7 +4170,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>43771</v>
       </c>
@@ -4186,7 +4190,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>43776</v>
       </c>
@@ -4206,7 +4210,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>43778</v>
       </c>
@@ -4226,7 +4230,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>43781</v>
       </c>
@@ -4246,7 +4250,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>43782</v>
       </c>
@@ -4266,7 +4270,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>43785</v>
       </c>
@@ -4286,7 +4290,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>43786</v>
       </c>
@@ -4306,7 +4310,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>43790</v>
       </c>
@@ -4326,7 +4330,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>43793</v>
       </c>
@@ -4346,7 +4350,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4354,7 +4358,7 @@
       <c r="E38" s="16"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4362,7 +4366,7 @@
       <c r="E39" s="16"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4370,7 +4374,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4378,7 +4382,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4405,14 +4409,14 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4424,12 +4428,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -4441,11 +4445,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="44">
         <v>43713</v>
       </c>
@@ -4485,7 +4489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>43714</v>
       </c>
@@ -4505,7 +4509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>43725</v>
       </c>
@@ -4525,7 +4529,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>43726</v>
       </c>
@@ -4545,7 +4549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="44">
         <v>43727</v>
       </c>
@@ -4565,7 +4569,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="44">
         <v>43728</v>
       </c>
@@ -4585,7 +4589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>87</v>
       </c>
@@ -4605,7 +4609,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="44">
         <v>43730</v>
       </c>
@@ -4625,7 +4629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>43735</v>
       </c>
@@ -4645,7 +4649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>88</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
         <v>43742</v>
       </c>
@@ -4685,7 +4689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>89</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>90</v>
       </c>
@@ -4725,7 +4729,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>92</v>
       </c>
@@ -4745,7 +4749,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>92</v>
       </c>
@@ -4765,7 +4769,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4773,7 +4777,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4781,7 +4785,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4789,7 +4793,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4797,7 +4801,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4805,7 +4809,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4813,7 +4817,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4821,7 +4825,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4829,7 +4833,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4837,7 +4841,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4845,7 +4849,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4853,7 +4857,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4861,7 +4865,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4869,7 +4873,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4877,7 +4881,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4885,7 +4889,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4893,7 +4897,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4901,7 +4905,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4924,17 +4928,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4946,12 +4950,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -4963,11 +4967,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4987,7 +4991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -5007,7 +5011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>43</v>
       </c>
@@ -5027,7 +5031,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
@@ -5047,7 +5051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
@@ -5067,7 +5071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
@@ -5087,7 +5091,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5095,7 +5099,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5103,7 +5107,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5111,7 +5115,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -5119,7 +5123,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5127,7 +5131,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -5135,7 +5139,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5143,7 +5147,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5151,7 +5155,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5159,7 +5163,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5167,7 +5171,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5175,7 +5179,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5183,7 +5187,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5191,7 +5195,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5199,7 +5203,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5207,7 +5211,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5215,7 +5219,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5223,7 +5227,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5231,7 +5235,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5239,7 +5243,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5247,7 +5251,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5255,7 +5259,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5263,7 +5267,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5271,7 +5275,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5279,7 +5283,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5287,7 +5291,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5295,7 +5299,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5303,7 +5307,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5327,17 +5331,17 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5349,12 +5353,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -5366,11 +5370,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5390,7 +5394,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -5410,7 +5414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43714</v>
       </c>
@@ -5430,7 +5434,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43715</v>
       </c>
@@ -5450,7 +5454,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>43717</v>
       </c>
@@ -5470,7 +5474,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>43725</v>
       </c>
@@ -5490,7 +5494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>43726</v>
       </c>
@@ -5510,7 +5514,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>43727</v>
       </c>
@@ -5530,7 +5534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>43728</v>
       </c>
@@ -5550,7 +5554,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>43730</v>
       </c>
@@ -5570,7 +5574,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
         <v>43735</v>
       </c>
@@ -5590,7 +5594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="30">
         <v>43738</v>
       </c>
@@ -5610,7 +5614,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>43739</v>
       </c>
@@ -5630,7 +5634,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>43739</v>
       </c>
@@ -5650,7 +5654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="30">
         <v>43742</v>
       </c>
@@ -5670,7 +5674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>43744</v>
       </c>
@@ -5690,7 +5694,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>43748</v>
       </c>
@@ -5710,7 +5714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="30">
         <v>43766</v>
       </c>
@@ -5730,7 +5734,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>43768</v>
       </c>
@@ -5750,7 +5754,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>43772</v>
       </c>
@@ -5770,7 +5774,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>43776</v>
       </c>
@@ -5790,7 +5794,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="30">
         <v>43779</v>
       </c>
@@ -5810,7 +5814,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A27" s="30">
         <v>43780</v>
       </c>
@@ -5830,7 +5834,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>43783</v>
       </c>
@@ -5850,15 +5854,27 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>43792</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="16">
+        <v>180</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5866,7 +5882,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5874,7 +5890,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5882,7 +5898,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5890,7 +5906,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5898,7 +5914,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5906,7 +5922,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5914,7 +5930,7 @@
       <c r="E36" s="16"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5922,7 +5938,7 @@
       <c r="E37" s="16"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5930,7 +5946,7 @@
       <c r="E38" s="16"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5938,7 +5954,7 @@
       <c r="E39" s="16"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5946,7 +5962,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5954,7 +5970,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5981,14 +5997,14 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
@@ -6000,12 +6016,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -6017,11 +6033,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6041,7 +6057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -6061,7 +6077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>43714</v>
       </c>
@@ -6081,7 +6097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>43725</v>
       </c>
@@ -6101,7 +6117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>43726</v>
       </c>
@@ -6121,7 +6137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>43727</v>
       </c>
@@ -6141,7 +6157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>67</v>
       </c>
@@ -6161,7 +6177,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>69</v>
       </c>
@@ -6181,7 +6197,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>71</v>
       </c>
@@ -6201,7 +6217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>73</v>
       </c>
@@ -6221,7 +6237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>74</v>
       </c>
@@ -6241,7 +6257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>75</v>
       </c>
@@ -6261,7 +6277,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>77</v>
       </c>
@@ -6281,7 +6297,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>80</v>
       </c>
@@ -6301,7 +6317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>80</v>
       </c>
@@ -6321,7 +6337,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>82</v>
       </c>
@@ -6341,7 +6357,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -6361,7 +6377,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>86</v>
       </c>
@@ -6381,7 +6397,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="30">
         <v>43764</v>
       </c>
@@ -6401,7 +6417,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="30">
         <v>43764</v>
       </c>
@@ -6421,7 +6437,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="30">
         <v>43774</v>
       </c>
@@ -6441,7 +6457,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>43777</v>
       </c>
@@ -6461,7 +6477,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>43778</v>
       </c>
@@ -6481,7 +6497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="30">
         <v>43778</v>
       </c>
@@ -6501,7 +6517,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6509,7 +6525,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6517,7 +6533,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6525,7 +6541,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6533,7 +6549,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6541,7 +6557,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6549,7 +6565,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6557,7 +6573,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6565,7 +6581,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6573,7 +6589,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6596,17 +6612,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="39.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6618,12 +6634,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -6635,11 +6651,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6659,7 +6675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>34</v>
       </c>
@@ -6679,7 +6695,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -6699,7 +6715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
@@ -6719,7 +6735,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
@@ -6739,7 +6755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
@@ -6759,7 +6775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>41</v>
       </c>
@@ -6779,7 +6795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6787,7 +6803,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6795,7 +6811,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6803,7 +6819,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6811,7 +6827,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6819,7 +6835,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6827,7 +6843,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6835,7 +6851,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6843,7 +6859,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6851,7 +6867,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6859,7 +6875,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6867,7 +6883,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6875,7 +6891,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6883,7 +6899,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6891,7 +6907,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6899,7 +6915,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6907,7 +6923,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -6915,7 +6931,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -6923,7 +6939,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -6931,7 +6947,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -6939,7 +6955,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -6947,7 +6963,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -6955,7 +6971,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -6963,7 +6979,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -6971,7 +6987,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -6979,7 +6995,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7007,26 +7023,26 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
         <v>13</v>
       </c>
@@ -7043,7 +7059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>49</v>
       </c>
@@ -7061,7 +7077,7 @@
       </c>
       <c r="E5" s="38"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>21</v>
       </c>
@@ -7081,7 +7097,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
@@ -7101,7 +7117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>20</v>
       </c>
@@ -7121,7 +7137,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>26</v>
       </c>
@@ -7141,7 +7157,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>28</v>
       </c>
@@ -7161,7 +7177,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>33</v>
       </c>
@@ -7181,7 +7197,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>55</v>
       </c>
@@ -7201,7 +7217,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>59</v>
       </c>
@@ -7221,7 +7237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -7241,7 +7257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>95</v>
       </c>
@@ -7261,7 +7277,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>99</v>
       </c>
@@ -7281,7 +7297,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>100</v>
       </c>
@@ -7301,7 +7317,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>103</v>
       </c>
@@ -7311,11 +7327,11 @@
       </c>
       <c r="C18" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A18,김혜민!E:E)+SUMIF('김백준(휴학)'!F:F,TOTAL!A18,'김백준(휴학)'!E:E)+SUMIF(박진근!F:F,TOTAL!A18,박진근!E:E)+SUMIF(이미정!F:F,TOTAL!A18,이미정!E:E)+SUMIF(정동연!F:F,TOTAL!A18,정동연!E:E)+SUMIF(탁재인!F:F,TOTAL!A18,탁재인!E:E)</f>
-        <v>2360</v>
+        <v>2540</v>
       </c>
       <c r="D18" s="37">
         <f t="shared" ref="D18" si="4">C18-B18</f>
-        <v>1760</v>
+        <v>1940</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
update_ change prefer/nonprefer brand, psp
</commit_message>
<xml_diff>
--- a/5조_PSP.xlsx
+++ b/5조_PSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongdong-yeon/Documents/GitHub/pumasi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1C3CFE8-FDD6-F242-8D3D-D75DD5246C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F377BC-6332-8246-B0BB-45022AEE419F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9560" yWindow="980" windowWidth="15660" windowHeight="13540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -5961,8 +5961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -6586,67 +6586,55 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="13">
+      <c r="A34" s="30">
         <v>43801</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="25">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C34" s="3">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="D34" s="8">
-        <v>0</v>
-      </c>
-      <c r="E34" s="16">
-        <v>110</v>
-      </c>
-      <c r="F34" s="4" t="s">
+      <c r="C34" s="25">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="D34" s="28">
+        <v>170</v>
+      </c>
+      <c r="E34" s="28">
+        <v>480</v>
+      </c>
+      <c r="F34" s="26" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="13">
-        <v>43801</v>
+        <v>43802</v>
       </c>
       <c r="B35" s="3">
-        <v>0.61111111111111105</v>
+        <v>0.70138888888888884</v>
       </c>
       <c r="C35" s="3">
-        <v>0.6875</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D35" s="8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E35" s="16">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="13">
-        <v>43801</v>
-      </c>
-      <c r="B36" s="3">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="D36" s="8">
-        <v>30</v>
-      </c>
-      <c r="E36" s="8">
-        <v>140</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="A36" s="13"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="4"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="8"/>
@@ -6654,7 +6642,7 @@
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="4"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="8"/>
@@ -7387,15 +7375,15 @@
       </c>
       <c r="B18" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A18,김혜민!D:D)+SUMIF('김백준(휴학)'!F:F,TOTAL!A18,'김백준(휴학)'!D:D)+SUMIF(박진근!F:F,TOTAL!A18,박진근!D:D)+SUMIF(이미정!F:F,TOTAL!A18,이미정!D:D)+SUMIF(정동연!F:F,TOTAL!A18,정동연!D:D)+SUMIF(탁재인!F:F,TOTAL!A18,탁재인!D:D)</f>
-        <v>1060</v>
+        <v>1230</v>
       </c>
       <c r="C18" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A18,김혜민!E:E)+SUMIF('김백준(휴학)'!F:F,TOTAL!A18,'김백준(휴학)'!E:E)+SUMIF(박진근!F:F,TOTAL!A18,박진근!E:E)+SUMIF(이미정!F:F,TOTAL!A18,이미정!E:E)+SUMIF(정동연!F:F,TOTAL!A18,정동연!E:E)+SUMIF(탁재인!F:F,TOTAL!A18,탁재인!E:E)</f>
-        <v>3890</v>
+        <v>4140</v>
       </c>
       <c r="D18" s="37">
         <f t="shared" ref="D18" si="4">C18-B18</f>
-        <v>2830</v>
+        <v>2910</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
psp, test case update
</commit_message>
<xml_diff>
--- a/5조_PSP.xlsx
+++ b/5조_PSP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeongdong-yeon/Documents/GitHub/pumasi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hye Min\Documents\GitHub\pumasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62724226-84DF-694F-9173-1BC2C4C7D881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04067692-67BB-4D9E-9340-106458253CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="980" windowWidth="15660" windowHeight="13540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="김혜민" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="탁재인" sheetId="6" r:id="rId6"/>
     <sheet name="TOTAL" sheetId="17" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1210,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="113">
   <si>
     <t>Table C16  Time Recording Log</t>
   </si>
@@ -2976,6 +2976,10 @@
       </rPr>
       <t>로직짜기</t>
     </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -2991,7 +2995,7 @@
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3159,7 +3163,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -3251,6 +3255,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - 강조색6" xfId="3" builtinId="50"/>
@@ -3639,20 +3644,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="11.75" customHeight="1">
+    <row r="1" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -3664,10 +3669,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="11.75" customHeight="1">
+    <row r="2" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
     </row>
-    <row r="3" spans="1:8" ht="11.75" customHeight="1">
+    <row r="3" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -3679,8 +3684,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="11.75" customHeight="1"/>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="28">
+    <row r="4" spans="1:8" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3700,7 +3705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -3721,7 +3726,7 @@
       </c>
       <c r="H6" s="21"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>43713</v>
       </c>
@@ -3742,7 +3747,7 @@
       </c>
       <c r="H7" s="21"/>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>43714</v>
       </c>
@@ -3762,7 +3767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>43715</v>
       </c>
@@ -3782,7 +3787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>43717</v>
       </c>
@@ -3802,7 +3807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>43725</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>43726</v>
       </c>
@@ -3842,7 +3847,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>43727</v>
       </c>
@@ -3862,7 +3867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
         <v>43728</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>43728</v>
       </c>
@@ -3902,7 +3907,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>43728</v>
       </c>
@@ -3922,7 +3927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>43730</v>
       </c>
@@ -3942,7 +3947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>43735</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>43736</v>
       </c>
@@ -3982,7 +3987,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
         <v>43736</v>
       </c>
@@ -4002,7 +4007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>43742</v>
       </c>
@@ -4022,7 +4027,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>43745</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>43745</v>
       </c>
@@ -4062,7 +4067,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>43747</v>
       </c>
@@ -4082,7 +4087,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>43748</v>
       </c>
@@ -4102,7 +4107,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>43749</v>
       </c>
@@ -4122,7 +4127,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>43764</v>
       </c>
@@ -4142,7 +4147,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>43764</v>
       </c>
@@ -4162,7 +4167,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>43771</v>
       </c>
@@ -4182,7 +4187,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>43776</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>43778</v>
       </c>
@@ -4222,7 +4227,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>43781</v>
       </c>
@@ -4242,7 +4247,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>43782</v>
       </c>
@@ -4262,7 +4267,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <v>43785</v>
       </c>
@@ -4282,7 +4287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <v>43786</v>
       </c>
@@ -4302,7 +4307,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>43790</v>
       </c>
@@ -4322,47 +4327,107 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1">
-      <c r="A37" s="13"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1">
-      <c r="A38" s="13"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1">
-      <c r="A39" s="13"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1">
-      <c r="A40" s="13"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1">
-      <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="13">
+        <v>43798</v>
+      </c>
+      <c r="B37" s="25">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="16">
+        <v>270</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="13">
+        <v>43799</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D38" s="8">
+        <v>30</v>
+      </c>
+      <c r="E38" s="16">
+        <v>210</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>43800</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0</v>
+      </c>
+      <c r="E39" s="16">
+        <v>420</v>
+      </c>
+      <c r="F39" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
+        <v>43802</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="8">
+        <v>30</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="47">
+        <v>43805</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D41" s="8">
+        <v>0</v>
+      </c>
+      <c r="E41" s="8">
+        <v>90</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4389,14 +4454,14 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4408,12 +4473,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -4425,11 +4490,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4449,7 +4514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="44">
         <v>43713</v>
       </c>
@@ -4469,7 +4534,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="44">
         <v>43714</v>
       </c>
@@ -4489,7 +4554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="44">
         <v>43725</v>
       </c>
@@ -4509,7 +4574,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="44">
         <v>43726</v>
       </c>
@@ -4529,7 +4594,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="44">
         <v>43727</v>
       </c>
@@ -4549,7 +4614,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="44">
         <v>43728</v>
       </c>
@@ -4569,7 +4634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>87</v>
       </c>
@@ -4589,7 +4654,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="44">
         <v>43730</v>
       </c>
@@ -4609,7 +4674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="44">
         <v>43735</v>
       </c>
@@ -4629,7 +4694,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
         <v>88</v>
       </c>
@@ -4649,7 +4714,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="44">
         <v>43742</v>
       </c>
@@ -4669,7 +4734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="45" t="s">
         <v>89</v>
       </c>
@@ -4689,7 +4754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>90</v>
       </c>
@@ -4709,7 +4774,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>92</v>
       </c>
@@ -4729,7 +4794,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>92</v>
       </c>
@@ -4749,7 +4814,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4757,7 +4822,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4765,7 +4830,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4773,7 +4838,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4781,7 +4846,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4789,7 +4854,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4797,7 +4862,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4805,7 +4870,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4813,7 +4878,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4821,7 +4886,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4829,7 +4894,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4837,7 +4902,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4845,7 +4910,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4853,7 +4918,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4861,7 +4926,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4869,7 +4934,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4877,7 +4942,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4885,7 +4950,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4912,13 +4977,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4930,12 +4995,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -4947,11 +5012,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -4971,7 +5036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -4991,7 +5056,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>43</v>
       </c>
@@ -5011,7 +5076,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
@@ -5031,7 +5096,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
@@ -5051,7 +5116,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
@@ -5071,7 +5136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -5079,7 +5144,7 @@
       <c r="E11" s="16"/>
       <c r="F11" s="18"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5087,7 +5152,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -5095,7 +5160,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -5103,7 +5168,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5111,7 +5176,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -5119,7 +5184,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -5127,7 +5192,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5135,7 +5200,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -5143,7 +5208,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -5151,7 +5216,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -5159,7 +5224,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5167,7 +5232,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5175,7 +5240,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5183,7 +5248,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5191,7 +5256,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5199,7 +5264,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5207,7 +5272,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -5215,7 +5280,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5223,7 +5288,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5231,7 +5296,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5239,7 +5304,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5247,7 +5312,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5255,7 +5320,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5263,7 +5328,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5271,7 +5336,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5279,7 +5344,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5287,7 +5352,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5310,18 +5375,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5333,12 +5398,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -5350,11 +5415,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -5374,7 +5439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -5394,7 +5459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>43714</v>
       </c>
@@ -5414,7 +5479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>43715</v>
       </c>
@@ -5434,7 +5499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
         <v>43717</v>
       </c>
@@ -5454,7 +5519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="31">
         <v>43725</v>
       </c>
@@ -5474,7 +5539,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>43726</v>
       </c>
@@ -5494,7 +5559,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
         <v>43727</v>
       </c>
@@ -5514,7 +5579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
         <v>43728</v>
       </c>
@@ -5534,7 +5599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
         <v>43730</v>
       </c>
@@ -5554,7 +5619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
         <v>43735</v>
       </c>
@@ -5574,7 +5639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
         <v>43738</v>
       </c>
@@ -5594,7 +5659,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>43739</v>
       </c>
@@ -5614,7 +5679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>43739</v>
       </c>
@@ -5634,7 +5699,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
         <v>43742</v>
       </c>
@@ -5654,7 +5719,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
         <v>43744</v>
       </c>
@@ -5674,7 +5739,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
         <v>43748</v>
       </c>
@@ -5694,7 +5759,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>43766</v>
       </c>
@@ -5714,7 +5779,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>43768</v>
       </c>
@@ -5734,7 +5799,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
         <v>43772</v>
       </c>
@@ -5754,7 +5819,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>43776</v>
       </c>
@@ -5774,7 +5839,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <v>43779</v>
       </c>
@@ -5794,7 +5859,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
         <v>43780</v>
       </c>
@@ -5814,7 +5879,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>43783</v>
       </c>
@@ -5834,7 +5899,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -5842,7 +5907,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -5850,7 +5915,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -5858,7 +5923,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5866,7 +5931,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -5874,7 +5939,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -5882,7 +5947,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -5890,7 +5955,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -5898,7 +5963,7 @@
       <c r="E36" s="16"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="13"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -5906,7 +5971,7 @@
       <c r="E37" s="16"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -5914,7 +5979,7 @@
       <c r="E38" s="16"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -5922,7 +5987,7 @@
       <c r="E39" s="16"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -5930,7 +5995,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -5938,7 +6003,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -5961,18 +6026,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>15</v>
       </c>
@@ -5984,12 +6049,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -6001,11 +6066,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6025,7 +6090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>43713</v>
       </c>
@@ -6045,7 +6110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>43714</v>
       </c>
@@ -6065,7 +6130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>43725</v>
       </c>
@@ -6085,7 +6150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>43726</v>
       </c>
@@ -6105,7 +6170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>43727</v>
       </c>
@@ -6125,7 +6190,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>67</v>
       </c>
@@ -6145,7 +6210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>69</v>
       </c>
@@ -6165,7 +6230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>71</v>
       </c>
@@ -6185,7 +6250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>73</v>
       </c>
@@ -6205,7 +6270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>74</v>
       </c>
@@ -6225,7 +6290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>75</v>
       </c>
@@ -6245,7 +6310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>77</v>
       </c>
@@ -6265,7 +6330,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>80</v>
       </c>
@@ -6285,7 +6350,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>80</v>
       </c>
@@ -6305,7 +6370,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>82</v>
       </c>
@@ -6325,7 +6390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>85</v>
       </c>
@@ -6345,7 +6410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>86</v>
       </c>
@@ -6365,7 +6430,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>43764</v>
       </c>
@@ -6385,7 +6450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
         <v>43764</v>
       </c>
@@ -6405,7 +6470,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
         <v>43774</v>
       </c>
@@ -6425,7 +6490,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>43777</v>
       </c>
@@ -6445,7 +6510,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>43778</v>
       </c>
@@ -6465,7 +6530,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <v>43778</v>
       </c>
@@ -6485,7 +6550,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>43785</v>
       </c>
@@ -6505,7 +6570,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
         <v>43791</v>
       </c>
@@ -6525,7 +6590,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="30">
         <v>43794</v>
       </c>
@@ -6545,7 +6610,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>43796</v>
       </c>
@@ -6565,7 +6630,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>43799</v>
       </c>
@@ -6585,7 +6650,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
         <v>43801</v>
       </c>
@@ -6605,7 +6670,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <v>43802</v>
       </c>
@@ -6625,7 +6690,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>43803</v>
       </c>
@@ -6645,7 +6710,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="30">
         <v>43803</v>
       </c>
@@ -6665,7 +6730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -6692,13 +6757,13 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -6710,12 +6775,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="14">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -6727,11 +6792,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="28">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -6751,7 +6816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>34</v>
       </c>
@@ -6771,7 +6836,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -6791,7 +6856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
@@ -6811,7 +6876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>39</v>
       </c>
@@ -6831,7 +6896,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
@@ -6851,7 +6916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>41</v>
       </c>
@@ -6871,7 +6936,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6879,7 +6944,7 @@
       <c r="E12" s="16"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6887,7 +6952,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6895,7 +6960,7 @@
       <c r="E14" s="16"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6903,7 +6968,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6911,7 +6976,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="14">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6919,7 +6984,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6927,7 +6992,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -6935,7 +7000,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="14">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -6943,7 +7008,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -6951,7 +7016,7 @@
       <c r="E21" s="16"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -6959,7 +7024,7 @@
       <c r="E22" s="16"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6967,7 +7032,7 @@
       <c r="E23" s="16"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6975,7 +7040,7 @@
       <c r="E24" s="16"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6983,7 +7048,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -6991,7 +7056,7 @@
       <c r="E26" s="16"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -6999,7 +7064,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -7007,7 +7072,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -7015,7 +7080,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -7023,7 +7088,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -7031,7 +7096,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7039,7 +7104,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -7047,7 +7112,7 @@
       <c r="E33" s="16"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -7055,7 +7120,7 @@
       <c r="E34" s="16"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -7063,7 +7128,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7071,7 +7136,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7099,26 +7164,26 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>13</v>
       </c>
@@ -7135,7 +7200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>49</v>
       </c>
@@ -7153,7 +7218,7 @@
       </c>
       <c r="E5" s="38"/>
     </row>
-    <row r="6" spans="1:5" ht="14">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>21</v>
       </c>
@@ -7173,7 +7238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
@@ -7193,7 +7258,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>20</v>
       </c>
@@ -7213,7 +7278,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>26</v>
       </c>
@@ -7233,7 +7298,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>28</v>
       </c>
@@ -7253,7 +7318,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>33</v>
       </c>
@@ -7273,7 +7338,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>55</v>
       </c>
@@ -7293,7 +7358,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
         <v>59</v>
       </c>
@@ -7313,7 +7378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>63</v>
       </c>
@@ -7333,7 +7398,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>95</v>
       </c>
@@ -7353,7 +7418,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>99</v>
       </c>
@@ -7363,17 +7428,17 @@
       </c>
       <c r="C16" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A16,김혜민!E:E)+SUMIF('김백준(휴학)'!F:F,TOTAL!A16,'김백준(휴학)'!E:E)+SUMIF(박진근!F:F,TOTAL!A16,박진근!E:E)+SUMIF(이미정!F:F,TOTAL!A16,이미정!E:E)+SUMIF(정동연!F:F,TOTAL!A16,정동연!E:E)+SUMIF(탁재인!F:F,TOTAL!A16,탁재인!E:E)</f>
-        <v>340</v>
+        <v>430</v>
       </c>
       <c r="D16" s="37">
         <f t="shared" ref="D16" si="2">C16-B16</f>
-        <v>290</v>
+        <v>380</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>100</v>
       </c>
@@ -7393,21 +7458,21 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A18,김혜민!D:D)+SUMIF('김백준(휴학)'!F:F,TOTAL!A18,'김백준(휴학)'!D:D)+SUMIF(박진근!F:F,TOTAL!A18,박진근!D:D)+SUMIF(이미정!F:F,TOTAL!A18,이미정!D:D)+SUMIF(정동연!F:F,TOTAL!A18,정동연!D:D)+SUMIF(탁재인!F:F,TOTAL!A18,탁재인!D:D)</f>
-        <v>1290</v>
+        <v>1320</v>
       </c>
       <c r="C18" s="37">
         <f>SUMIF(김혜민!F:F,TOTAL!A18,김혜민!E:E)+SUMIF('김백준(휴학)'!F:F,TOTAL!A18,'김백준(휴학)'!E:E)+SUMIF(박진근!F:F,TOTAL!A18,박진근!E:E)+SUMIF(이미정!F:F,TOTAL!A18,이미정!E:E)+SUMIF(정동연!F:F,TOTAL!A18,정동연!E:E)+SUMIF(탁재인!F:F,TOTAL!A18,탁재인!E:E)</f>
-        <v>4320</v>
+        <v>5250</v>
       </c>
       <c r="D18" s="37">
         <f t="shared" ref="D18" si="4">C18-B18</f>
-        <v>3030</v>
+        <v>3930</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>104</v>

</xml_diff>